<commit_message>
Added Hindi language support
</commit_message>
<xml_diff>
--- a/dummy_data.xlsx
+++ b/dummy_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\College\MNNIT\NCC Paper Generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\College\MNNIT\NCC Paper Generator\Github\NCC-Paper-Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AD8598-4147-4A40-9EDB-799E0672A682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141856A9-C526-47F8-9DEF-622F9BE6CA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22510" uniqueCount="2732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22510" uniqueCount="2733">
   <si>
     <t>Question id</t>
   </si>
@@ -8463,12 +8463,15 @@
   <si>
     <t xml:space="preserve">What is difference between " Ek File &amp; Single File? And what is 'Ek Line'. </t>
   </si>
+  <si>
+    <t>जो होने वाला है वो होकर ही रहता है और जो नहीं होने वाला वह कभी नहीं होता</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8498,6 +8501,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Akshar Unicode"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -8519,9 +8527,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8828,8 +8839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J2532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2493" workbookViewId="0">
-      <selection activeCell="A2502" sqref="A2502:XFD2502"/>
+    <sheetView tabSelected="1" topLeftCell="A2424" workbookViewId="0">
+      <selection activeCell="H2422" sqref="H2422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -86309,7 +86320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2422" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2422" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A2422" t="s">
         <v>2441</v>
       </c>
@@ -86319,8 +86330,8 @@
       <c r="C2422" t="s">
         <v>35</v>
       </c>
-      <c r="D2422" s="1" t="s">
-        <v>2620</v>
+      <c r="D2422" s="2" t="s">
+        <v>2732</v>
       </c>
       <c r="E2422" t="s">
         <v>13</v>
@@ -86341,7 +86352,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2423" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="2423" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A2423" t="s">
         <v>2442</v>
       </c>
@@ -86351,8 +86362,8 @@
       <c r="C2423" t="s">
         <v>35</v>
       </c>
-      <c r="D2423" s="1" t="s">
-        <v>2621</v>
+      <c r="D2423" s="2" t="s">
+        <v>2732</v>
       </c>
       <c r="E2423" t="s">
         <v>13</v>
@@ -86373,7 +86384,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2424" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="2424" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A2424" t="s">
         <v>2443</v>
       </c>
@@ -86383,8 +86394,8 @@
       <c r="C2424" t="s">
         <v>35</v>
       </c>
-      <c r="D2424" s="1" t="s">
-        <v>2622</v>
+      <c r="D2424" s="2" t="s">
+        <v>2732</v>
       </c>
       <c r="E2424" t="s">
         <v>13</v>
@@ -86405,7 +86416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2425" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2425" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A2425" t="s">
         <v>2444</v>
       </c>
@@ -86415,8 +86426,8 @@
       <c r="C2425" t="s">
         <v>35</v>
       </c>
-      <c r="D2425" s="1" t="s">
-        <v>2623</v>
+      <c r="D2425" s="2" t="s">
+        <v>2732</v>
       </c>
       <c r="E2425" t="s">
         <v>13</v>
@@ -86437,7 +86448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2426" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2426" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A2426" t="s">
         <v>2445</v>
       </c>
@@ -86447,8 +86458,8 @@
       <c r="C2426" t="s">
         <v>35</v>
       </c>
-      <c r="D2426" s="1" t="s">
-        <v>2624</v>
+      <c r="D2426" s="2" t="s">
+        <v>2732</v>
       </c>
       <c r="E2426" t="s">
         <v>13</v>
@@ -86469,7 +86480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2427" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2427" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A2427" t="s">
         <v>2446</v>
       </c>
@@ -86479,8 +86490,8 @@
       <c r="C2427" t="s">
         <v>35</v>
       </c>
-      <c r="D2427" s="1" t="s">
-        <v>2625</v>
+      <c r="D2427" s="2" t="s">
+        <v>2732</v>
       </c>
       <c r="E2427" t="s">
         <v>13</v>
@@ -86501,7 +86512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2428" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2428" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A2428" t="s">
         <v>2447</v>
       </c>
@@ -86511,8 +86522,8 @@
       <c r="C2428" t="s">
         <v>35</v>
       </c>
-      <c r="D2428" s="1" t="s">
-        <v>2626</v>
+      <c r="D2428" s="2" t="s">
+        <v>2732</v>
       </c>
       <c r="E2428" t="s">
         <v>13</v>
@@ -86533,7 +86544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2429" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2429" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A2429" t="s">
         <v>2448</v>
       </c>
@@ -86543,8 +86554,8 @@
       <c r="C2429" t="s">
         <v>35</v>
       </c>
-      <c r="D2429" s="1" t="s">
-        <v>2627</v>
+      <c r="D2429" s="2" t="s">
+        <v>2732</v>
       </c>
       <c r="E2429" t="s">
         <v>13</v>
@@ -86565,7 +86576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2430" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2430" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A2430" t="s">
         <v>2449</v>
       </c>
@@ -86575,8 +86586,8 @@
       <c r="C2430" t="s">
         <v>35</v>
       </c>
-      <c r="D2430" s="1" t="s">
-        <v>2628</v>
+      <c r="D2430" s="2" t="s">
+        <v>2732</v>
       </c>
       <c r="E2430" t="s">
         <v>13</v>
@@ -86597,7 +86608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2431" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2431" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A2431" t="s">
         <v>2450</v>
       </c>
@@ -86607,8 +86618,8 @@
       <c r="C2431" t="s">
         <v>35</v>
       </c>
-      <c r="D2431" s="1" t="s">
-        <v>2629</v>
+      <c r="D2431" s="2" t="s">
+        <v>2732</v>
       </c>
       <c r="E2431" t="s">
         <v>13</v>
@@ -86725,7 +86736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2435" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="2435" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A2435" t="s">
         <v>2454</v>
       </c>
@@ -87205,7 +87216,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2450" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="2450" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A2450" t="s">
         <v>2469</v>
       </c>
@@ -87333,7 +87344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2454" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="2454" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A2454" t="s">
         <v>2473</v>
       </c>
@@ -87653,7 +87664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2464" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="2464" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A2464" t="s">
         <v>2483</v>
       </c>
@@ -87909,7 +87920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2472" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="2472" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A2472" t="s">
         <v>2491</v>
       </c>
@@ -88964,5 +88975,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>